<commit_message>
updating hardware sample XLSX
</commit_message>
<xml_diff>
--- a/data/Hardware/degthatnetwork-hardwareassetlist.xlsx
+++ b/data/Hardware/degthatnetwork-hardwareassetlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dalebingham/soteria/OpenRMFPro/RMF-Files/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AFADE1-B42D-8742-9C92-84D368D03206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84C7D4-FF02-0E43-A5D0-F98C9B67E654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3320" yWindow="3740" windowWidth="29400" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HardwareListing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
   <si>
     <t>Operating System</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>desktop team</t>
+  </si>
+  <si>
+    <t>linux, server team</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,7 +493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -492,13 +501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -509,9 +518,10 @@
     <col min="4" max="8" width="40" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
     <col min="10" max="10" width="60" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -542,8 +552,11 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -572,8 +585,11 @@
       <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -602,8 +618,11 @@
       <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -632,8 +651,11 @@
       <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -662,8 +684,11 @@
       <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -692,8 +717,11 @@
       <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -722,8 +750,11 @@
       <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -752,8 +783,9 @@
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -782,8 +814,9 @@
       <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -812,6 +845,7 @@
       <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating sample data used
</commit_message>
<xml_diff>
--- a/data/Hardware/degthatnetwork-hardwareassetlist.xlsx
+++ b/data/Hardware/degthatnetwork-hardwareassetlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dalebingham/soteria/OpenRMFPro/RMF-Files/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84C7D4-FF02-0E43-A5D0-F98C9B67E654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD3086D-8C44-5945-80EF-723BE91437C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="3740" windowWidth="29400" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21460" yWindow="11180" windowWidth="29400" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HardwareListing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Operating System</t>
   </si>
@@ -119,6 +119,57 @@
   </si>
   <si>
     <t>linux, server team</t>
+  </si>
+  <si>
+    <t>IP Addresses</t>
+  </si>
+  <si>
+    <t>MAC Addresses</t>
+  </si>
+  <si>
+    <t>10.10.25.17</t>
+  </si>
+  <si>
+    <t>00:0C:29:88:C9:7D</t>
+  </si>
+  <si>
+    <t>10.10.30.22</t>
+  </si>
+  <si>
+    <t>10.10.30.20</t>
+  </si>
+  <si>
+    <t>10.10.25.11</t>
+  </si>
+  <si>
+    <t>10.10.25.67</t>
+  </si>
+  <si>
+    <t>10.10.30.34</t>
+  </si>
+  <si>
+    <t>10.10.25.119</t>
+  </si>
+  <si>
+    <t>10.10.30.220, 10.10.30.222</t>
+  </si>
+  <si>
+    <t>00:0C:33:88:C9:7D</t>
+  </si>
+  <si>
+    <t>00:0C:29:33:C9:7D</t>
+  </si>
+  <si>
+    <t>00:0C:45:88:C9:7D</t>
+  </si>
+  <si>
+    <t>00:0C:29:88:C9:7A</t>
+  </si>
+  <si>
+    <t>00:0C:29:49:C9:7D</t>
+  </si>
+  <si>
+    <t>00:0C:25:88:C9:7D</t>
   </si>
 </sst>
 </file>
@@ -177,15 +228,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -205,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,27 +558,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="100" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="50" customWidth="1"/>
-    <col min="10" max="10" width="60" customWidth="1"/>
-    <col min="11" max="11" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="30" style="2" customWidth="1"/>
+    <col min="2" max="2" width="100" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1"/>
+    <col min="4" max="8" width="40" style="2" customWidth="1"/>
+    <col min="9" max="9" width="50" style="2" customWidth="1"/>
+    <col min="10" max="10" width="60" style="2" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -555,297 +615,353 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="L7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="2"/>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>